<commit_message>
parser finished, output files deleted
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1028f8d26f624cd18d39-my.sharepoint.com/personal/ozan_yetkin_metu_edu_tr/Documents/Desktop/Projects/pdf-parser/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_E45E3CD67C19EAD342160B0F4319FD47512CA01A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4F2F6B9-262D-4370-AB39-A801182B8C2D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="223">
   <si>
     <t>name</t>
   </si>
@@ -28,6 +34,9 @@
     <t>word_count</t>
   </si>
   <si>
+    <t>cities</t>
+  </si>
+  <si>
     <t>abdul aziz omar</t>
   </si>
   <si>
@@ -37,6 +46,9 @@
     <t>ahmet ege sert</t>
   </si>
   <si>
+    <t>ahmet emre yetkin</t>
+  </si>
+  <si>
     <t>ahmet musab ayan</t>
   </si>
   <si>
@@ -49,6 +61,9 @@
     <t>amna rizwan</t>
   </si>
   <si>
+    <t>asel sude aydin</t>
+  </si>
+  <si>
     <t>aslihan umay ongun</t>
   </si>
   <si>
@@ -67,6 +82,9 @@
     <t>berkay aydin</t>
   </si>
   <si>
+    <t>beyzanur gok</t>
+  </si>
+  <si>
     <t>bilge esra sahin</t>
   </si>
   <si>
@@ -88,12 +106,27 @@
     <t>doga dolay</t>
   </si>
   <si>
+    <t>duru senol</t>
+  </si>
+  <si>
+    <t>ebru cetin</t>
+  </si>
+  <si>
+    <t>ece kayhan</t>
+  </si>
+  <si>
     <t>ecem nur saygili</t>
   </si>
   <si>
+    <t>eda abdullahzade</t>
+  </si>
+  <si>
     <t>ege kiratli</t>
   </si>
   <si>
+    <t>elif cetin</t>
+  </si>
+  <si>
     <t>elif ceyhan</t>
   </si>
   <si>
@@ -118,6 +151,9 @@
     <t>farah habash</t>
   </si>
   <si>
+    <t>fatemeh saraei</t>
+  </si>
+  <si>
     <t>furkan durkut</t>
   </si>
   <si>
@@ -145,6 +181,9 @@
     <t>hilal koca</t>
   </si>
   <si>
+    <t>idil iris elkiran</t>
+  </si>
+  <si>
     <t>idil lal gulmen</t>
   </si>
   <si>
@@ -154,12 +193,30 @@
     <t>iraz serra canbay</t>
   </si>
   <si>
+    <t>ismail can ozdemir</t>
+  </si>
+  <si>
     <t>kerem ulukan</t>
   </si>
   <si>
+    <t>lara satir</t>
+  </si>
+  <si>
+    <t>leyli afandiyeva</t>
+  </si>
+  <si>
     <t>maryam sadikhzada</t>
   </si>
   <si>
+    <t>mehmet derin incekas</t>
+  </si>
+  <si>
+    <t>mehmet fatih cenebasi</t>
+  </si>
+  <si>
+    <t>mehmet gurcu</t>
+  </si>
+  <si>
     <t>melis ceren ozdemir</t>
   </si>
   <si>
@@ -169,9 +226,15 @@
     <t>merve mecife onder</t>
   </si>
   <si>
+    <t>muhammed bahadir pehlivan</t>
+  </si>
+  <si>
     <t>muhammet teymiyye oztok</t>
   </si>
   <si>
+    <t>murat kagan gulec</t>
+  </si>
+  <si>
     <t>nisa gezer</t>
   </si>
   <si>
@@ -193,9 +256,6 @@
     <t>onur ordek</t>
   </si>
   <si>
-    <t>others</t>
-  </si>
-  <si>
     <t>ozge altas</t>
   </si>
   <si>
@@ -220,15 +280,33 @@
     <t>selin gulay</t>
   </si>
   <si>
+    <t>selin sahin</t>
+  </si>
+  <si>
     <t>senem bekar</t>
   </si>
   <si>
+    <t>sila ozdemir</t>
+  </si>
+  <si>
     <t>sule karakas</t>
   </si>
   <si>
     <t>tolga ocal</t>
   </si>
   <si>
+    <t>ulku keskin</t>
+  </si>
+  <si>
+    <t>umit kahveci</t>
+  </si>
+  <si>
+    <t>utku kan</t>
+  </si>
+  <si>
+    <t>yagmur kaya</t>
+  </si>
+  <si>
     <t>yagmur unay</t>
   </si>
   <si>
@@ -238,17 +316,386 @@
     <t>zeynep asli birinci</t>
   </si>
   <si>
+    <t>zeynep aydin</t>
+  </si>
+  <si>
     <t>zeynep kurd</t>
   </si>
   <si>
     <t>zeynep nur saglam</t>
+  </si>
+  <si>
+    <t>zulal ari</t>
+  </si>
+  <si>
+    <t>'İstanbul'</t>
+  </si>
+  <si>
+    <t>'Ankara'</t>
+  </si>
+  <si>
+    <t>'Moscow'</t>
+  </si>
+  <si>
+    <t>'İzmir'</t>
+  </si>
+  <si>
+    <t>'Chita'</t>
+  </si>
+  <si>
+    <t>'Oslo'</t>
+  </si>
+  <si>
+    <t>'Ardahan'</t>
+  </si>
+  <si>
+    <t>'Ontario'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Toronto'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Ankara'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Murray'</t>
+  </si>
+  <si>
+    <t>'Cairo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ANKARA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Havana'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Konya'</t>
+  </si>
+  <si>
+    <t>'Wilson'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Moscow'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Stockholm'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'İzmir'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Samara'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'London'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Karachi'</t>
+  </si>
+  <si>
+    <t>'Quito'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Eskişehir'</t>
+  </si>
+  <si>
+    <t>'Hamburg'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'KONYA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Sevilla'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Lyon'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Sydney'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Aydın'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Penza'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Bursa'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Aswan'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Riyadh'</t>
+  </si>
+  <si>
+    <t>'Gediz'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Novi'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Irkutsk'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'İstanbul'</t>
+  </si>
+  <si>
+    <t>'Nevşehir'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Muğla'</t>
+  </si>
+  <si>
+    <t>'Ayvalık'</t>
+  </si>
+  <si>
+    <t>'Yakutsk'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Denizli'</t>
+  </si>
+  <si>
+    <t>'Tampere'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Bangkok'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Kingston'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Portland'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Jamaica'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Bandar'</t>
+  </si>
+  <si>
+    <t>'Victoria'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Melbourne'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Incheon'</t>
+  </si>
+  <si>
+    <t>'Mexico'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Veracruz'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Dhahran'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Cambridge'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Jeddah'</t>
+  </si>
+  <si>
+    <t>'Helsinki'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Yazd'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Warsaw'</t>
+  </si>
+  <si>
+    <t>'Singapore'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Malacca'</t>
+  </si>
+  <si>
+    <t>'Samara'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Kahramanmaraş'</t>
+  </si>
+  <si>
+    <t>'Miami'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Florida'</t>
+  </si>
+  <si>
+    <t>'Bay'</t>
+  </si>
+  <si>
+    <t>'Berlin'</t>
+  </si>
+  <si>
+    <t>'Kastamonu'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Valencia'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Erzurum'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Kütahya'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Barcelona'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Adana'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Beaufort'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Porto'</t>
+  </si>
+  <si>
+    <t>'Lafayette'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Indianapolis'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Chicago'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Antalya'</t>
+  </si>
+  <si>
+    <t>'Şanlıurfa'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Oslo'</t>
+  </si>
+  <si>
+    <t>'Stockholm'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Baku'</t>
+  </si>
+  <si>
+    <t>'Beaufort'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Johannesburg'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Casablanca'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Delhi'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Mumbai'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Berlin'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Jakarta'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Mexico'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Doha'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Sivas'</t>
+  </si>
+  <si>
+    <t>'Kayseri'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Amsterdam'</t>
+  </si>
+  <si>
+    <t>'Baku'</t>
+  </si>
+  <si>
+    <t>'otaru'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Menderes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Sapporo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Van'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Adelaide'</t>
+  </si>
+  <si>
+    <t>'Phoenix'</t>
+  </si>
+  <si>
+    <t>'Antananarivo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Tehran'</t>
+  </si>
+  <si>
+    <t>'Richmond'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Columbia'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Vancouver'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Ulsan'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Helsinki'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Singapore'</t>
+  </si>
+  <si>
+    <t>'Riyadh'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Artvin'</t>
+  </si>
+  <si>
+    <t>'Calgary'</t>
+  </si>
+  <si>
+    <t>'Warsaw'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Ordu'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Santiago'</t>
+  </si>
+  <si>
+    <t>'London'</t>
+  </si>
+  <si>
+    <t>'Samsun'</t>
+  </si>
+  <si>
+    <t>'Linhares'</t>
+  </si>
+  <si>
+    <t>'Antofagasta'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,17 +747,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,7 +813,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,9 +845,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,6 +897,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -598,14 +1090,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,13 +1112,16 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>19</v>
@@ -635,13 +1132,19 @@
       <c r="E2">
         <v>1775</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>13</v>
@@ -652,13 +1155,20 @@
       <c r="E3">
         <v>1938</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="2"/>
+      <c r="G3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>28</v>
@@ -669,1195 +1179,2223 @@
       <c r="E4">
         <v>2254</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>324</v>
+        <v>405</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>1648</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>38</v>
+        <v>300</v>
       </c>
       <c r="E6">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>2472</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>1669</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E8">
-        <v>1267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1650</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="I8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E9">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>1267</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+      <c r="J9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="E10">
-        <v>1983</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1887</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E11">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>1748</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" t="s">
+        <v>122</v>
+      </c>
+      <c r="K11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D12">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E12">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>1983</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="D13">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E13">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>2023</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="H13" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E14">
-        <v>2053</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>1258</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
         <v>17</v>
       </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>18</v>
-      </c>
       <c r="E15">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>1639</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D16">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E16">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>2053</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="K16" t="s">
+        <v>111</v>
+      </c>
+      <c r="L16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>495</v>
       </c>
       <c r="E17">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>1966</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="H17" t="s">
+        <v>132</v>
+      </c>
+      <c r="K17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
         <v>18</v>
       </c>
-      <c r="D18">
-        <v>396</v>
-      </c>
       <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>1684</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D19">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="E19">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>1545</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="I19" t="s">
+        <v>119</v>
+      </c>
+      <c r="L19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D20">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E20">
-        <v>2699</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>1434</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="E21">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>1786</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" t="s">
+        <v>137</v>
+      </c>
+      <c r="K21" t="s">
+        <v>111</v>
+      </c>
+      <c r="N21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D22">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E22">
-        <v>3121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>1539</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D23">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E23">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>2699</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D24">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E24">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>810</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D25">
-        <v>16</v>
+        <v>392</v>
       </c>
       <c r="E25">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>1509</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D26">
-        <v>53</v>
+        <v>880</v>
       </c>
       <c r="E26">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>1818</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <v>38</v>
+        <v>544</v>
       </c>
       <c r="E27">
-        <v>1963</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>1762</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="D28">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E28">
-        <v>1927</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>3121</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="E29">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>1701</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E30">
-        <v>2210</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>1991</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" t="s">
+        <v>147</v>
+      </c>
+      <c r="K30" t="s">
+        <v>148</v>
+      </c>
+      <c r="M30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C31">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D31">
-        <v>98</v>
+        <v>216</v>
       </c>
       <c r="E31">
-        <v>3306</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>1527</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E32">
-        <v>2362</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>1616</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C33">
+        <v>12</v>
+      </c>
+      <c r="D33">
         <v>16</v>
       </c>
-      <c r="D33">
-        <v>52</v>
-      </c>
       <c r="E33">
-        <v>1937</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>1021</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J33" t="s">
+        <v>111</v>
+      </c>
+      <c r="K33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D34">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E34">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>2200</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="H34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D35">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E35">
-        <v>1744</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>1963</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D36">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E36">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>1927</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E37">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>1529</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D38">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E38">
-        <v>1745</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>2210</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" t="s">
+        <v>118</v>
+      </c>
+      <c r="J38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D39">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="E39">
-        <v>2099</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>3306</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" t="s">
+        <v>156</v>
+      </c>
+      <c r="H39" t="s">
+        <v>157</v>
+      </c>
+      <c r="J39" t="s">
+        <v>139</v>
+      </c>
+      <c r="K39" t="s">
+        <v>158</v>
+      </c>
+      <c r="L39" t="s">
+        <v>111</v>
+      </c>
+      <c r="N39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C40">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D40">
-        <v>35</v>
+        <v>364</v>
       </c>
       <c r="E40">
-        <v>1885</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>1654</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C41">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E41">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>2362</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C42">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D42">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E42">
-        <v>1613</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>1937</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I42" t="s">
+        <v>111</v>
+      </c>
+      <c r="J42" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D43">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E43">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>1223</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C44">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D44">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E44">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>1744</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J44" t="s">
+        <v>111</v>
+      </c>
+      <c r="K44" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C45">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D45">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E45">
-        <v>2929</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>1662</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="H45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D46">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E46">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>1376</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C47">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D47">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E47">
-        <v>1727</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>1745</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D48">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E48">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>2099</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H48" t="s">
+        <v>111</v>
+      </c>
+      <c r="J48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C49">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E49">
-        <v>1914</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>1885</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H49" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C50">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D50">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E50">
-        <v>1559</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>2415</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" t="s">
+        <v>173</v>
+      </c>
+      <c r="I50" t="s">
+        <v>125</v>
+      </c>
+      <c r="M50" t="s">
+        <v>111</v>
+      </c>
+      <c r="N50" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C51">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D51">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E51">
-        <v>2312</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>1605</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" t="s">
+        <v>111</v>
+      </c>
+      <c r="H51" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C52">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D52">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E52">
-        <v>2753</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>1613</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" t="s">
+        <v>176</v>
+      </c>
+      <c r="H52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C53">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D53">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="E53">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>1890</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G53" t="s">
+        <v>179</v>
+      </c>
+      <c r="I53" t="s">
+        <v>180</v>
+      </c>
+      <c r="J53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C54">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D54">
-        <v>31</v>
+        <v>272</v>
       </c>
       <c r="E54">
-        <v>1818</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>2232</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" t="s">
+        <v>110</v>
+      </c>
+      <c r="H54" t="s">
+        <v>181</v>
+      </c>
+      <c r="J54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C55">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D55">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E55">
-        <v>1840</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>1695</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C56">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D56">
-        <v>35</v>
+        <v>595</v>
       </c>
       <c r="E56">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>1660</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H56" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C57">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D57">
-        <v>72</v>
+        <v>884</v>
       </c>
       <c r="E57">
-        <v>1887</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>2304</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H57" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C58">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D58">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E58">
-        <v>2415</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>2929</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G58" t="s">
+        <v>185</v>
+      </c>
+      <c r="H58" t="s">
+        <v>135</v>
+      </c>
+      <c r="I58" t="s">
+        <v>187</v>
+      </c>
+      <c r="J58" t="s">
+        <v>188</v>
+      </c>
+      <c r="L58" t="s">
+        <v>189</v>
+      </c>
+      <c r="M58" t="s">
+        <v>190</v>
+      </c>
+      <c r="N58" t="s">
+        <v>191</v>
+      </c>
+      <c r="O58" t="s">
+        <v>192</v>
+      </c>
+      <c r="P58" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D59">
-        <v>10</v>
+        <v>480</v>
       </c>
       <c r="E59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>1978</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="H59" t="s">
+        <v>181</v>
+      </c>
+      <c r="J59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C60">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D60">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="E60">
-        <v>1901</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>1332</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C61">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D61">
-        <v>43</v>
+        <v>1100</v>
       </c>
       <c r="E61">
-        <v>2072</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>2308</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C62">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D62">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E62">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>1399</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C63">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D63">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E63">
-        <v>2156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>1727</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" t="s">
+        <v>116</v>
+      </c>
+      <c r="H63" t="s">
+        <v>191</v>
+      </c>
+      <c r="I63" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C64">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D64">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="E64">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>1890</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C65">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D65">
-        <v>21</v>
+        <v>492</v>
       </c>
       <c r="E65">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>1844</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C66">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D66">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E66">
-        <v>1672</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>1914</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G66" t="s">
+        <v>115</v>
+      </c>
+      <c r="K66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C67">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D67">
-        <v>52</v>
+        <v>648</v>
       </c>
       <c r="E67">
-        <v>2172</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>1671</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" t="s">
+        <v>111</v>
+      </c>
+      <c r="H67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C68">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D68">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E68">
-        <v>1491</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>1559</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C69">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D69">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E69">
-        <v>2732</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+        <v>2312</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I69" t="s">
+        <v>200</v>
+      </c>
+      <c r="J69" t="s">
+        <v>201</v>
+      </c>
+      <c r="M69" t="s">
+        <v>202</v>
+      </c>
+      <c r="N69" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C70">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D70">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E70">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>2753</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G70" t="s">
+        <v>185</v>
+      </c>
+      <c r="I70" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C71">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D71">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E71">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+        <v>1733</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H71" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C72">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D72">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E72">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+        <v>1818</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C73">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D73">
         <v>38</v>
       </c>
       <c r="E73">
-        <v>2644</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>1840</v>
+      </c>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74">
+        <v>24</v>
+      </c>
+      <c r="D74">
+        <v>35</v>
+      </c>
+      <c r="E74">
+        <v>1307</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J74" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>10</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76">
+        <v>16</v>
+      </c>
+      <c r="D76">
+        <v>37</v>
+      </c>
+      <c r="E76">
+        <v>1901</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="C74">
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77">
+        <v>19</v>
+      </c>
+      <c r="D77">
+        <v>43</v>
+      </c>
+      <c r="E77">
+        <v>2072</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G77" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78">
+        <v>24</v>
+      </c>
+      <c r="D78">
+        <v>49</v>
+      </c>
+      <c r="E78">
+        <v>2019</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G78" t="s">
+        <v>139</v>
+      </c>
+      <c r="K78" t="s">
+        <v>208</v>
+      </c>
+      <c r="M78" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79">
+        <v>20</v>
+      </c>
+      <c r="D79">
+        <v>43</v>
+      </c>
+      <c r="E79">
+        <v>2156</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G79" t="s">
+        <v>210</v>
+      </c>
+      <c r="H79" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>54</v>
+      </c>
+      <c r="E80">
+        <v>1542</v>
+      </c>
+      <c r="F80" s="2"/>
+      <c r="G80" t="s">
+        <v>211</v>
+      </c>
+      <c r="H80" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81">
+        <v>7</v>
+      </c>
+      <c r="D81">
+        <v>21</v>
+      </c>
+      <c r="E81">
+        <v>1320</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G81" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82">
+        <v>14</v>
+      </c>
+      <c r="D82">
+        <v>50</v>
+      </c>
+      <c r="E82">
+        <v>1672</v>
+      </c>
+      <c r="F82" s="2"/>
+      <c r="G82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H82" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83">
+        <v>380</v>
+      </c>
+      <c r="E83">
+        <v>1582</v>
+      </c>
+      <c r="F83" s="2"/>
+      <c r="G83" t="s">
+        <v>120</v>
+      </c>
+      <c r="I83" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84">
+        <v>11</v>
+      </c>
+      <c r="D84">
+        <v>52</v>
+      </c>
+      <c r="E84">
+        <v>2172</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85">
+        <v>12</v>
+      </c>
+      <c r="D85">
+        <v>240</v>
+      </c>
+      <c r="E85">
+        <v>1181</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86">
+        <v>20</v>
+      </c>
+      <c r="D86">
+        <v>38</v>
+      </c>
+      <c r="E86">
+        <v>1491</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="G86" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>90</v>
+      </c>
+      <c r="C87">
+        <v>38</v>
+      </c>
+      <c r="D87">
+        <v>36</v>
+      </c>
+      <c r="E87">
+        <v>2732</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H87" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88">
+        <v>41</v>
+      </c>
+      <c r="D88">
+        <v>5084</v>
+      </c>
+      <c r="E88">
+        <v>347</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89">
+        <v>17</v>
+      </c>
+      <c r="D89">
+        <v>578</v>
+      </c>
+      <c r="E89">
+        <v>2117</v>
+      </c>
+      <c r="F89" s="2"/>
+      <c r="H89" t="s">
+        <v>217</v>
+      </c>
+      <c r="I89" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>93</v>
+      </c>
+      <c r="C90">
+        <v>23</v>
+      </c>
+      <c r="D90">
+        <v>1196</v>
+      </c>
+      <c r="E90">
+        <v>1991</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H90" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>94</v>
+      </c>
+      <c r="C91">
+        <v>12</v>
+      </c>
+      <c r="D91">
+        <v>240</v>
+      </c>
+      <c r="E91">
+        <v>1390</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>95</v>
+      </c>
+      <c r="C92">
+        <v>11</v>
+      </c>
+      <c r="D92">
+        <v>43</v>
+      </c>
+      <c r="E92">
+        <v>1380</v>
+      </c>
+      <c r="F92" s="2"/>
+      <c r="G92" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>96</v>
+      </c>
+      <c r="C93">
+        <v>12</v>
+      </c>
+      <c r="D93">
+        <v>33</v>
+      </c>
+      <c r="E93">
+        <v>1271</v>
+      </c>
+      <c r="F93" s="2"/>
+      <c r="G93" t="s">
+        <v>120</v>
+      </c>
+      <c r="I93" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>97</v>
+      </c>
+      <c r="C94">
+        <v>6</v>
+      </c>
+      <c r="D94">
+        <v>30</v>
+      </c>
+      <c r="E94">
+        <v>1275</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C95">
+        <v>9</v>
+      </c>
+      <c r="D95">
+        <v>270</v>
+      </c>
+      <c r="E95">
+        <v>1477</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G95" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>99</v>
+      </c>
+      <c r="C96">
+        <v>20</v>
+      </c>
+      <c r="D96">
+        <v>38</v>
+      </c>
+      <c r="E96">
+        <v>2644</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G96" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+      <c r="C97">
         <v>8</v>
       </c>
-      <c r="D74">
+      <c r="D97">
         <v>23</v>
       </c>
-      <c r="E74">
+      <c r="E97">
         <v>1442</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G97" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>101</v>
+      </c>
+      <c r="C98">
+        <v>9</v>
+      </c>
+      <c r="D98">
+        <v>342</v>
+      </c>
+      <c r="E98">
+        <v>1670</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>